<commit_message>
Keywords (Fotos -> Stichworte)
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Data/fotos_1.xlsx
+++ b/Excel_Mapping/Data/fotos_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rossinière VS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architektur; Personen</t>
   </si>
   <si>
     <t xml:space="preserve">images/hunziker/Hunziker_AV_0004_001.jpg</t>
@@ -500,8 +503,8 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -658,20 +661,23 @@
       <c r="K2" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="L2" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="M2" s="0" t="n">
         <v>186</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>29</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>7.08259</v>
@@ -680,10 +686,10 @@
         <v>46.46782</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>